<commit_message>
Change 550 takeoff throttle
</commit_message>
<xml_diff>
--- a/STM32F4/gps_pid_550.xlsx
+++ b/STM32F4/gps_pid_550.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jngeun\Desktop\KUAV\STM32F4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66FDDB91-B425-4368-9B20-D7E8F6A41885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621D44D3-95DA-46C4-BB41-F6422320A749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>outer</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,6 +110,63 @@
   <si>
     <t>d
 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외란이 작용되는 축은 수렴이 안되서 밀려나감
+외란이 없는 축은 오버슛이 되서 진동이 발생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드론이 너무 많이 기울어서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점점 발산이 되고 모터값이 튕김</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발산은 이전보다 덜하고 모터값이 튀는 현상은 그대로 유지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3m 진폭으로 왔다갔다 오버슛이 생기고 모터가 튀는 현상은 그대로 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모터가 튀는 현상은 그대로이고 진폭은 1.5m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모터 튀는 현상 그래도 있고 바람이 불면 밀리다가 5미터쯤 다시 돌아오고 오버슛은 없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왔다갔다 하면서 발산이 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바람을 잘 견디지만 오버슛 심함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바람을 견디지 못하고 오버슛 심함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제어가 약해서 못 감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발산의 정도는 작지만 오버슛을 하지는 않음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모터 튀는 현상 없고 타깃으로 전혀 가지 못함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바람이 불 때 목표로 가지 못 함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -159,16 +216,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,6 +233,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,33 +526,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="63.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="78.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
       <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -514,259 +580,551 @@
       <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="F3" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8" t="s">
+    <row r="4" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A4" s="8"/>
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="C4" s="5"/>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>6</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8" t="s">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A5" s="8"/>
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
+      <c r="C5" s="5"/>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>6</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="45.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="3" t="s">
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" ht="45.6" x14ac:dyDescent="0.4">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="45.6" x14ac:dyDescent="0.4">
-      <c r="A7" s="3"/>
-      <c r="B7" s="8" t="s">
+    <row r="7" spans="1:15" ht="45.6" x14ac:dyDescent="0.4">
+      <c r="A7" s="8"/>
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
+      <c r="F7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="I7" s="2">
+        <v>6</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:15" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A8" s="8"/>
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="2">
+        <v>6</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="F9" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="2">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I11" s="2">
+        <v>4</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I12" s="2">
+        <v>4</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="I13" s="2">
+        <v>4</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K13" s="2">
+        <v>2</v>
+      </c>
+      <c r="L13" s="10"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F15" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+      <c r="F16" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="6:14" x14ac:dyDescent="0.4">
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
+      <c r="F17" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>4</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="L17" s="10"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="6:14" x14ac:dyDescent="0.4">
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="F18" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>4</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="L18" s="10"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="6:14" x14ac:dyDescent="0.4">
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
+      <c r="F19" s="2">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
     <row r="20" spans="6:14" x14ac:dyDescent="0.4">
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="F20" s="2">
+        <v>20</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
     <row r="21" spans="6:14" x14ac:dyDescent="0.4">
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2">
+        <v>100</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="6:14" x14ac:dyDescent="0.4">
+      <c r="L32" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>